<commit_message>
Added a bit of results
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Linear reduced</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t xml:space="preserve">  - </t>
+  </si>
+  <si>
+    <t>Explicit mode</t>
   </si>
 </sst>
 </file>
@@ -402,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F5"/>
+  <dimension ref="B1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -416,9 +419,10 @@
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="15.88671875" customWidth="1"/>
     <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="2:8">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -434,13 +438,16 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:8">
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:8">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -457,7 +464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:8">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -474,7 +481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:8">
       <c r="B5" t="s">
         <v>8</v>
       </c>

</xml_diff>